<commit_message>
update data set and openai model
</commit_message>
<xml_diff>
--- a/src/shared/data-set.xlsx
+++ b/src/shared/data-set.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Documents\fine-tuning-openai\src\shared\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPeU\munibot_openai\munibot-fine-tuning-openai-backend\src\shared\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1675A9-A15A-4415-8792-8E775B31655A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21921E25-9652-4597-AA21-C82C3C9770F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="596" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QnAs" sheetId="1" r:id="rId1"/>
+    <sheet name="seet-Muni" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="448">
   <si>
     <t>Question</t>
   </si>
@@ -1034,6 +1035,336 @@
   </si>
   <si>
     <t>¿Qué debo hacer si olvidé la clave, Nombre de Usuario o si deseo cambiarlo para acceder a Home Banking?</t>
+  </si>
+  <si>
+    <t>El administrado puede acceder a la información documentaria fedateada de la institución.</t>
+  </si>
+  <si>
+    <t>¿ Quiero hacer mis tramites a donde debo presentar mis documentos?</t>
+  </si>
+  <si>
+    <t>Si tiene que presentar algun documento acerquese a mesa de partes de la Municipalidad Provincial de San Martin.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para realizar la solicitud de certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para el certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para el certificado de documentos fedateados es PA19732E20.</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de certificados de documentos fedateados, debes presentar una solicitud simple dirigida al responsable de otorgar la información (Secretario(a) General).</t>
+  </si>
+  <si>
+    <t>¿En qué consiste el certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo del certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la reconsideración del certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la reconsideración del certificado de documentos fedateados es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la reconsideración del certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la reconsideración del certificado de documentos fedateados es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la apelación del certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la apelación del certificado de documentos fedateados es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la apelación del certificado de documentos fedateados?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la apelación del certificado de documentos fedateados es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para el certificado de documentos fedateados es PE1027380A2.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para realizar la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la licencia de funcionamiento para cambio de giro, debes presentar una Declaración jurada para informar el cambio de giro.</t>
+  </si>
+  <si>
+    <t>¿En qué consiste la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>Procedimiento a través del cual, toda persona natural o jurídica que cuenta con licencia de funcionamiento para establecimientos calificados con nivel de riesgo bajo o medio, y que decide cambiar de giro de negocio, puede realizar en el establecimiento obras de refacción y/o acondicionamiento, a fin de adecuar sus instalaciones al nuevo giro, sin afectar las condiciones de seguridad, ni incrementar la clasificación del nivel de riesgo a alto o muy alto. El procedimiento es de aprobación automática.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo de la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la reconsideración de la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para reconsideración de la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la licencia de funcionamiento para cambio de giro es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la apelación de la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la apelación de la licencia de funcionamiento para cambio de giro es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la apelación de la licencia de funcionamiento para cambio de giro?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la apelación de la licencia de funcionamiento para cambio de giro es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la licencia de funcionamiento para cambio de giro es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para la nulidad de registro de matrimonio es PA1973129F.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para realizar la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la nulidad de registro de matrimonio, debes presentar 1. una sentencia y oficio expedida por el Juez. 2.Recibo de derecho de pago.</t>
+  </si>
+  <si>
+    <t>¿En qué consiste la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>Pedir la nulidad matrimonial supone un proceso relativamente directo para disolver un matrimonio. Sin embargo, a veces tiene la complejidad de que es mucho más complicado de probar en comparación a un divorcio. Al declararse la nulidad matrimonial, las partes regresan a su estado civil inicial.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo de la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la reconsideración de la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la nulidad de registro de matrimonio es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para reconsideración de la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la nulidad de registro de matrimonio es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la apelación de la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la apelación de la nulidad de registro de matrimonio?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la apelación de la nulidad de registro de matrimonio es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para la inscripción y ejecución de matrimonio civil es PA1973F15F.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para realizar la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la inscripción y ejecución de matrimonio civil, debes presentar 1.- Solicitud de Matrimonio. 2.- Partida de Nacimiento originales de cada contrayente (Actualizada). 3.- Presentar copia legalizada del documento de Identidad de cada contrayente. 4.- Certificado Médico de cada contrayente expedido preferentemente por el Hospital o Centro de Salud. 5.- Certificado de soltería de cada contrayente. 6.- Certificado Domiciliario de cada contrayente. 7.- Publicación del Edicto Matrimonial en el Diario Oficial de la Región (adjuntar la publicación en el expediente). Nota:Presentar la solicitud matrimonial 15 días antes de la ceremonia, considerando 2 Testigos mayores de edad.</t>
+  </si>
+  <si>
+    <t>¿En qué consiste la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>El administrado podrá tramitar su inscripción y ejecución de Matrimonio Civil en los canales de atención de la Entidad.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo de la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la reconsideración de la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la inscripción y ejecución de matrimonio civil es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para reconsideración de la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la inscripción y ejecución de matrimonio civil es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la apelación de la inscripción y ejecución de matrimonio civil?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la apelación de la inscripción y ejecución de matrimonio civil es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para el reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para el reconocimiento de nacimiento (con posterioridad) es PA19739815.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para el reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de reconocimiento de nacimiento (con posterioridad), debes presentar 1.Reconocimiento voluntario derecho de pago y DNI de los padres. 2.Reconocimiento notarial-Escritura Pública. 3.- Reconocimiento Judicial.-Oficio y Resolución Judicial. 4.- Recibo de derecho de pago.</t>
+  </si>
+  <si>
+    <t>¿En qué consiste el reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>Una vez asentada la nueva partida o acta de nacimiento, el registrador o funcionario encargado del Registro Nacional de Identificación y Estado Civil o de las Oficinas Registrales autorizadas por este, sólo expedirá, bajo responsabilidad, copia certificada de la nueva partida o acta de nacimiento, salvo mandato judicial en contrario.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo del reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para el reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para el reconocimiento de nacimiento (con posterioridad) es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para reconsideración de el reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para el reconocimiento de nacimiento (con posterioridad) es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para el reconocimiento de nacimiento (con posterioridad)?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para la inscripción de matrimonio realizado en el extranjero es PA19738007.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la inscripción de matrimonio realizado en el extranjero, debes presentar 1.-Partida de Matrimonio realizado en el Extranjero. 2.- Sentencia y Oficio que expide el Juez.</t>
+  </si>
+  <si>
+    <t>¿En qué consiste la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>El peruano que contrajera matrimonio en el extranjero puede solicitar la inscripción en cualquiera de las Oficinas Registrales Consulares del país donde se realizó dicho acto. A este efecto presentará copia certificada del acta matrimonial, traducida en caso de estar en idioma extranjero.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo de la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la inscripción de matrimonio realizado en el extranjero es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para reconsideración de la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la inscripción de matrimonio realizado en el extranjero es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para el la inscripción de matrimonio realizado en el extranjero es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la inscripción de matrimonio realizado en el extranjero?</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación de la inscripción de matrimonio realizado en el extranjero es de S/ 32.30.</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación del certificado de documentos fedateados es gratuito.</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación de la licencia de funcionamiento para cambio de giro es de S/25.90.</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación de la nulidad de registro de matrimonio es de S/29.10.</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación del Formulario de inscripción - Monto - S/ 10.00, Derecho de Matrimonio Civil - En la Municipalidad en horas de trabajo - Monto S/ 80.60, Derecho de Matrimonio Civil - En la Municipalidad fuera del horario de trabajo - Monto S/ 107.20, Derecho de Matrimonio Civil - A domicilio en horas de trabajo - Monto S/ 115.40, Derecho de Matrimonio Civil - A domicilio fuera del horario de trabajo - Monto S/ 142.70</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación del reconocimiento de nacimiento (con posterioridad) es de S/ 26.00</t>
+  </si>
+  <si>
+    <t>¿Cuál es el código del procedimiento para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>El código de procedimiento para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones) es PA1973E443.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el procedimiento para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones), debes presentar 1.- Sentencia y Oficio que expide el Juez. 2.- Rectificación por Escritura Pública. 3.- Recibo de derecho de pago.</t>
+  </si>
+  <si>
+    <t>¿En qué consiste la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>Para la rectificación de los datos de las actas registrales.</t>
+  </si>
+  <si>
+    <t>¿Cuánto es el costo de la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación de la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones) es de S/ 24.20</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de presentación para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones) es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para reconsideración de la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>El plazo máximo de respuesta para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones) es de 30 días hábiles.</t>
+  </si>
+  <si>
+    <t>El plazo máximo de presentación para el la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones) es de 15 días hábiles.</t>
+  </si>
+  <si>
+    <t>¿Cuál es el plazo máximo de respuesta para la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones)?</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la inscripción de matrimonio realizado en el extranjero, debes presentar:\n\n1.-Partida de Matrimonio realizado en el Extranjero. :\n\n2.- Sentencia y Oficio que expide el Juez.</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la rectificación e inscripción judicial (matrimonio, defunción, nacimiento, divorcio, Adopciones), debes presentar :\n\n1.- Sentencia y Oficio que expide el Juez. :\n\n2.- Rectificación por Escritura Pública. :\n\n3.- Recibo de derecho de pago.</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la inscripción y ejecución de matrimonio civil, debes presentar :\n\n1.- Solicitud de Matrimonio. :\n\n2.- Partida de Nacimiento originales de cada contrayente (Actualizada). :\n\n3.- Presentar copia legalizada del documento de Identidad de cada contrayente. :\n\n 4.- Certificado Médico de cada contrayente expedido preferentemente por el Hospital o Centro de Salud. :\n\n5.- Certificado de soltería de cada contrayente. :\n\n6.- Certificado Domiciliario de cada contrayente. :\n\n7.- Publicación del Edicto Matrimonial en el Diario Oficial de la Región (adjuntar la publicación en el expediente). :\n\nNota:Presentar la solicitud matrimonial 15 días antes de la ceremonia, considerando 2 Testigos mayores de edad.</t>
+  </si>
+  <si>
+    <t>Para realizar el procedimiento de la nulidad de registro de matrimonio, debes presentar :\n\n1. una sentencia y oficio expedida por el Juez. :\n\n2.Recibo de derecho de pago.</t>
+  </si>
+  <si>
+    <t>El costo por derecho de tramitación del Formulario de inscripción - Monto - S/ 10.00, :\n\nDerecho de Matrimonio Civil - En la Municipalidad en horas de trabajo - Monto S/ 80.60, :\n\nDerecho de Matrimonio Civil - En la Municipalidad fuera del horario de trabajo - Monto S/ 107.20, :\n\nDerecho de Matrimonio Civil - A domicilio en horas de trabajo - Monto S/ 115.40, :\n\nDerecho de Matrimonio Civil - A domicilio fuera del horario de trabajo - Monto S/ 142.70</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1507,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1356,6 +1687,54 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1517,10 +1896,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1876,1402 +2262,2324 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B192"/>
+  <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A214" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A173" sqref="A173:B230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="63.44140625" customWidth="1"/>
+    <col min="1" max="1" width="134.6640625" customWidth="1"/>
     <col min="2" max="2" width="139.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>77</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>79</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>81</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="A45" t="s">
         <v>84</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>90</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>91</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>102</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>104</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>90</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>106</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>108</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>112</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>114</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>119</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>121</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>122</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>124</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>126</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="70" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>127</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>130</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="73" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>131</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="74" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="75" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>133</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>135</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="77" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>137</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="79" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>141</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="80" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>145</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>146</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>150</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>152</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="86" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>158</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>160</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="90" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>162</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>164</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="92" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>168</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>170</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>171</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="96" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>172</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>174</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>176</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="99" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>178</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>179</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="101" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>181</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="102" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>183</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="103" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>185</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="104" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>187</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="105" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>189</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="106" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>190</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>192</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="108" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>193</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="109" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>195</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="110" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>197</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="111" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>199</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="112" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>200</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="113" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>201</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="114" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>202</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="115" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
         <v>203</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="116" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>204</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="117" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
         <v>206</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="118" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>208</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="119" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>210</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="120" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>211</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="121" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>213</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="122" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
         <v>215</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="123" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
         <v>217</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
         <v>219</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="125" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>337</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="126" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>222</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="127" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>224</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="128" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>225</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="129" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>227</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="130" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>228</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="131" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>229</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="132" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>231</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="133" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>233</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="134" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>235</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="135" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
         <v>237</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="136" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>238</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="137" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>240</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="138" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>242</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="139" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>243</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="140" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
         <v>244</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="141" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
         <v>246</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="142" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>248</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="143" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
         <v>249</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="144" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
         <v>251</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="145" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>253</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="146" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="1" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>255</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="147" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>257</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="148" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="1" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>259</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="149" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>261</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="150" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>262</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="151" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>263</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="152" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>265</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="153" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
         <v>267</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="154" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>269</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="155" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>271</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="156" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>272</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="157" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
         <v>273</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="158" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
         <v>274</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="159" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="1" t="s">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
         <v>276</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="160" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
         <v>278</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="161" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
         <v>279</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="162" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A162" t="s">
         <v>281</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="163" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A163" t="s">
         <v>283</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="164" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
         <v>284</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="165" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
         <v>286</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="166" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" t="s">
         <v>287</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="167" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="1" t="s">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A167" t="s">
         <v>289</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="168" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
         <v>290</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="169" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" t="s">
         <v>291</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="170" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="1" t="s">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" t="s">
         <v>292</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="171" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="172" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="173" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="174" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="175" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="176" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="177" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="178" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="179" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="180" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="181" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="182" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="183" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="184" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="185" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="186" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="187" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="188" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="189" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="190" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="191" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="192" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A172" s="2"/>
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B173" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A174" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B174" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A175" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B175" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A176" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B176" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B177" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B178" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B179" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B180" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B181" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B182" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B183" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B184" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B185" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B186" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B187" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B188" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B189" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="B190" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B191" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="B192" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B193" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B194" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B195" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="B196" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B197" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="B198" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B199" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="B200" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B201" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="B202" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="B203" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="B204" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="B205" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="B206" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B207" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="B208" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="B209" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="B210" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="B211" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="B212" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B213" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B214" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="B215" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="B216" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="B217" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B218" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219" s="8" t="s">
+        <v>419</v>
+      </c>
+      <c r="B219" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="B220" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B221" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="B222" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="B223" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="B224" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="B225" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="B226" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B227" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="B228" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B229" t="s">
+        <v>440</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551BCA70-979F-45CF-854D-D7E3F894E78A}">
+  <dimension ref="A1:B58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="91.6640625" customWidth="1"/>
+    <col min="2" max="2" width="179.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B3" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>346</v>
+      </c>
+      <c r="B6" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>347</v>
+      </c>
+      <c r="B7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>349</v>
+      </c>
+      <c r="B8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>353</v>
+      </c>
+      <c r="B10" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B11" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>359</v>
+      </c>
+      <c r="B13" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>362</v>
+      </c>
+      <c r="B15" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>363</v>
+      </c>
+      <c r="B16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>365</v>
+      </c>
+      <c r="B17" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>367</v>
+      </c>
+      <c r="B18" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B21" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>376</v>
+      </c>
+      <c r="B22" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>377</v>
+      </c>
+      <c r="B23" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>379</v>
+      </c>
+      <c r="B24" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>381</v>
+      </c>
+      <c r="B25" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>384</v>
+      </c>
+      <c r="B27" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>386</v>
+      </c>
+      <c r="B28" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>388</v>
+      </c>
+      <c r="B29" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>390</v>
+      </c>
+      <c r="B30" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>393</v>
+      </c>
+      <c r="B32" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>395</v>
+      </c>
+      <c r="B33" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>396</v>
+      </c>
+      <c r="B34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>398</v>
+      </c>
+      <c r="B35" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>400</v>
+      </c>
+      <c r="B36" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>402</v>
+      </c>
+      <c r="B37" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>404</v>
+      </c>
+      <c r="B38" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>405</v>
+      </c>
+      <c r="B39" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>407</v>
+      </c>
+      <c r="B40" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>405</v>
+      </c>
+      <c r="B41" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>409</v>
+      </c>
+      <c r="B42" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>410</v>
+      </c>
+      <c r="B43" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>412</v>
+      </c>
+      <c r="B44" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>414</v>
+      </c>
+      <c r="B45" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>416</v>
+      </c>
+      <c r="B46" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>417</v>
+      </c>
+      <c r="B47" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>417</v>
+      </c>
+      <c r="B49" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>422</v>
+      </c>
+      <c r="B50" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>429</v>
+      </c>
+      <c r="B51" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>431</v>
+      </c>
+      <c r="B52" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>433</v>
+      </c>
+      <c r="B53" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>435</v>
+      </c>
+      <c r="B54" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>437</v>
+      </c>
+      <c r="B55" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>439</v>
+      </c>
+      <c r="B56" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>437</v>
+      </c>
+      <c r="B57" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>442</v>
+      </c>
+      <c r="B58" t="s">
+        <v>440</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>